<commit_message>
adding v2 outputs (crashed midway through MCMC, but with burnin =.4, looks good; intial shorter run failed to converge)
</commit_message>
<xml_diff>
--- a/src/copiesPerLocus_toSetup_swapping_etc.xlsx
+++ b/src/copiesPerLocus_toSetup_swapping_etc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlrothfels/Box Sync/R_Python_etal/git_repositories/homologizer/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4131E901-9342-7149-8FCD-ABF706B1AF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61672C6-D9F5-494C-AE2F-8D6F2A6F3445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="2160" windowWidth="30760" windowHeight="17920" xr2:uid="{AE534D98-65A7-4D43-BDD4-51ADCD2EEBC6}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>Fixed this -- _A was swapping with _A</t>
   </si>
   <si>
-    <t>Followup script?</t>
-  </si>
-  <si>
     <t>Do another analysis with a new tip created here, and see if it helps? (do model comparison with original version?)</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>Added to the swapping</t>
+  </si>
+  <si>
+    <t>v2 script</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -688,13 +688,13 @@
         <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
         <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1136,7 +1136,7 @@
         <v>60</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>66</v>
@@ -1156,7 +1156,7 @@
         <v>60</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>66</v>
@@ -1225,7 +1225,7 @@
         <v>64</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1248,7 +1248,7 @@
         <v>64</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1402,10 +1402,10 @@
         <v>61</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1422,10 +1422,10 @@
         <v>61</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1484,10 +1484,10 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
         <v>73</v>
-      </c>
-      <c r="F42" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:8">

</xml_diff>